<commit_message>
Hoang check ket qua danh gia => Chuc nang QuanLiXe
</commit_message>
<xml_diff>
--- a/trunk/Process/PhanCongDot3.xlsx
+++ b/trunk/Process/PhanCongDot3.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>3.3 Quản lý thông tin Trọng Tải
 - Phụ trách: Nhất Anh</t>
@@ -250,6 +250,9 @@
     <t>4. Mọi khó khăn, nên căn cứ vào phân công và lường trước để kịp thời giải quyết. Yêu cầu tương tác 
 mọi lúc có thể nêu có vấn đề phát sinh. Mục tiêu quan trọng nhất phải là đáp ứng &gt; 70% công việc 
 trước Deadline</t>
+  </si>
+  <si>
+    <t>70% (Xong 2/3 Chức năng)</t>
   </si>
 </sst>
 </file>
@@ -371,15 +374,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -400,40 +397,46 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -732,7 +735,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -746,13 +749,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="26.25" customHeight="1">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
     </row>
     <row r="2" spans="1:5" ht="28.5">
       <c r="A2" s="5" t="s">
@@ -772,183 +775,185 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="29.25">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
+      <c r="D3" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="14"/>
     </row>
     <row r="4" spans="1:5" ht="30">
-      <c r="A4" s="30"/>
-      <c r="B4" s="11" t="s">
+      <c r="A4" s="29"/>
+      <c r="B4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
     </row>
     <row r="5" spans="1:5" ht="30">
-      <c r="A5" s="30"/>
-      <c r="B5" s="11" t="s">
+      <c r="A5" s="29"/>
+      <c r="B5" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
     </row>
     <row r="6" spans="1:5" ht="30">
-      <c r="A6" s="30"/>
-      <c r="B6" s="11" t="s">
+      <c r="A6" s="29"/>
+      <c r="B6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
     </row>
     <row r="7" spans="1:5" ht="30">
-      <c r="A7" s="30"/>
-      <c r="B7" s="17" t="s">
+      <c r="A7" s="29"/>
+      <c r="B7" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
     </row>
     <row r="8" spans="1:5" ht="30">
-      <c r="A8" s="30"/>
-      <c r="B8" s="17" t="s">
+      <c r="A8" s="29"/>
+      <c r="B8" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
     </row>
     <row r="9" spans="1:5" ht="30">
-      <c r="A9" s="30"/>
-      <c r="B9" s="17" t="s">
+      <c r="A9" s="29"/>
+      <c r="B9" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
     </row>
     <row r="10" spans="1:5" ht="30">
-      <c r="A10" s="30"/>
-      <c r="B10" s="11" t="s">
+      <c r="A10" s="29"/>
+      <c r="B10" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
     </row>
     <row r="11" spans="1:5" ht="30">
-      <c r="A11" s="30"/>
-      <c r="B11" s="11" t="s">
+      <c r="A11" s="29"/>
+      <c r="B11" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
     </row>
     <row r="12" spans="1:5" ht="30">
-      <c r="A12" s="30"/>
-      <c r="B12" s="11" t="s">
+      <c r="A12" s="29"/>
+      <c r="B12" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
     </row>
     <row r="13" spans="1:5" ht="29.25">
-      <c r="A13" s="29" t="s">
+      <c r="A13" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
     </row>
     <row r="14" spans="1:5" ht="30">
-      <c r="A14" s="30"/>
-      <c r="B14" s="17" t="s">
+      <c r="A14" s="29"/>
+      <c r="B14" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
     </row>
     <row r="15" spans="1:5" s="4" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A15" s="29" t="s">
+      <c r="A15" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
     </row>
     <row r="16" spans="1:5" ht="30">
-      <c r="A16" s="29"/>
-      <c r="B16" s="14" t="s">
+      <c r="A16" s="28"/>
+      <c r="B16" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
     </row>
     <row r="17" spans="1:5" ht="30">
-      <c r="A17" s="29"/>
-      <c r="B17" s="14" t="s">
+      <c r="A17" s="28"/>
+      <c r="B17" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="24" t="s">
+      <c r="A20" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="24"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="27"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="19"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="22" t="s">
@@ -956,31 +961,31 @@
       </c>
       <c r="B21" s="22"/>
       <c r="C21" s="22"/>
-      <c r="D21" s="28"/>
+      <c r="D21" s="20"/>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="25" t="s">
+      <c r="A22" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="25"/>
-      <c r="C22" s="25"/>
-      <c r="D22" s="28"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="20"/>
     </row>
     <row r="23" spans="1:5" ht="30" customHeight="1">
-      <c r="A23" s="23" t="s">
+      <c r="A23" s="24" t="s">
         <v>42</v>
       </c>
       <c r="B23" s="22"/>
       <c r="C23" s="22"/>
-      <c r="D23" s="28"/>
+      <c r="D23" s="20"/>
     </row>
     <row r="24" spans="1:5" ht="51.75" customHeight="1">
-      <c r="A24" s="26" t="s">
+      <c r="A24" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="25"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="28"/>
+      <c r="B24" s="23"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -1015,32 +1020,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="28.5" customHeight="1">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="21" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="30">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="30" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="30">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="10"/>
+      <c r="B3" s="31"/>
     </row>
     <row r="4" spans="1:2" ht="30">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="10"/>
+      <c r="B4" s="31"/>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1"/>

</xml_diff>

<commit_message>
Hoang check danh gia ket qua theo tien do cho TuanAnh
</commit_message>
<xml_diff>
--- a/trunk/Process/PhanCongDot3.xlsx
+++ b/trunk/Process/PhanCongDot3.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
   <si>
     <t>3.3 Quản lý thông tin Trọng Tải
 - Phụ trách: Nhất Anh</t>
@@ -735,7 +735,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -797,7 +797,9 @@
       <c r="C4" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="8"/>
+      <c r="D4" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="E4" s="8"/>
     </row>
     <row r="5" spans="1:5" ht="30">

</xml_diff>

<commit_message>
Da them noi dung
</commit_message>
<xml_diff>
--- a/trunk/Process/PhanCongDot3.xlsx
+++ b/trunk/Process/PhanCongDot3.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
   <si>
     <t>3.3 Quản lý thông tin Trọng Tải
 - Phụ trách: Nhất Anh</t>
@@ -253,6 +253,9 @@
   </si>
   <si>
     <t>70% (Xong 2/3 Chức năng)</t>
+  </si>
+  <si>
+    <t>75%(Chưa làm phần GUI )</t>
   </si>
 </sst>
 </file>
@@ -734,8 +737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -821,7 +824,9 @@
       <c r="C6" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="8"/>
+      <c r="D6" s="8" t="s">
+        <v>51</v>
+      </c>
       <c r="E6" s="8"/>
     </row>
     <row r="7" spans="1:5" ht="30">

</xml_diff>